<commit_message>
Added new tasks and deleted old task files.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$120</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Project Blog</t>
   </si>
   <si>
-    <t>Gantt Chart</t>
-  </si>
-  <si>
     <t>Videos</t>
   </si>
   <si>
@@ -397,6 +394,30 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Battery Performance Specs</t>
+  </si>
+  <si>
+    <t>Battery performance - arm motion</t>
+  </si>
+  <si>
+    <t>Battery performance - drivetrain motion</t>
+  </si>
+  <si>
+    <t>Battery performance - baseline</t>
+  </si>
+  <si>
+    <t>Battery performance - arm on, not moving</t>
+  </si>
+  <si>
+    <t>Arm/Camera Calibration (Kinect)</t>
+  </si>
+  <si>
+    <t>Figure out why cRIO voltage reads 0 and fix</t>
+  </si>
+  <si>
+    <t>PC Power Supply auto-boot</t>
   </si>
 </sst>
 </file>
@@ -438,7 +459,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="33">
     <dxf>
       <fill>
         <patternFill>
@@ -470,13 +491,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -484,115 +498,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -613,15 +519,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -633,65 +533,163 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -989,10 +987,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <pane ySplit="585" activePane="bottomLeft"/>
+      <selection activeCell="A60" sqref="A60"/>
+      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,16 +1016,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
         <v>123</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>124</v>
-      </c>
-      <c r="H1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1">
@@ -1033,20 +1033,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <v>14</v>
       </c>
+      <c r="E2" t="str">
+        <f>IFERROR(VLOOKUP(C2,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F2" t="b">
-        <f>ISERROR(MATCH(A2,C$2:C$113,0))</f>
+        <f>ISERROR(MATCH(A2,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <f>AND(NOT(G2),F2,IF(D2&lt;&gt;"",VLOOKUP(D2,A$2:G$113,7),TRUE))</f>
+        <f>AND(NOT(G2),F2,IF(D2&lt;&gt;"",VLOOKUP(D2,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1055,20 +1059,24 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>14</v>
       </c>
+      <c r="E3" t="str">
+        <f>IFERROR(VLOOKUP(C3,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F3" t="b">
-        <f t="shared" ref="F3:F66" si="0">ISERROR(MATCH(A3,C$2:C$113,0))</f>
+        <f>ISERROR(MATCH(A3,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <f t="shared" ref="H3:H66" si="1">AND(NOT(G3),F3,IF(D3&lt;&gt;"",VLOOKUP(D3,A$2:G$113,7),TRUE))</f>
+        <f>AND(NOT(G3),F3,IF(D3&lt;&gt;"",VLOOKUP(D3,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1077,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -1085,15 +1093,19 @@
       <c r="D4">
         <v>68</v>
       </c>
+      <c r="E4" t="str">
+        <f>IFERROR(VLOOKUP(C4,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F4" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A4,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G4),F4,IF(D4&lt;&gt;"",VLOOKUP(D4,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1102,20 +1114,24 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>13</v>
       </c>
+      <c r="E5" t="str">
+        <f>IFERROR(VLOOKUP(C5,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F5" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A5,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G5),F5,IF(D5&lt;&gt;"",VLOOKUP(D5,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1124,20 +1140,24 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>13</v>
       </c>
+      <c r="E6" t="str">
+        <f>IFERROR(VLOOKUP(C6,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F6" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A6,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="H6" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G6),F6,IF(D6&lt;&gt;"",VLOOKUP(D6,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1146,20 +1166,24 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7">
         <v>13</v>
       </c>
+      <c r="E7" t="str">
+        <f>IFERROR(VLOOKUP(C7,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F7" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A7,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
       <c r="H7" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G7),F7,IF(D7&lt;&gt;"",VLOOKUP(D7,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1168,45 +1192,53 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>12</v>
       </c>
+      <c r="E8" t="str">
+        <f>IFERROR(VLOOKUP(C8,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F8" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A8,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="H8" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <f>AND(NOT(G8),F8,IF(D8&lt;&gt;"",VLOOKUP(D8,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="E9" t="str">
+        <f>IFERROR(VLOOKUP(C9,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F9" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A9,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="e">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G9),F9,IF(D9&lt;&gt;"",VLOOKUP(D9,A$2:G$120,7),TRUE))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1215,20 +1247,24 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>12</v>
       </c>
+      <c r="E10" t="str">
+        <f>IFERROR(VLOOKUP(C10,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F10" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A10,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G10),F10,IF(D10&lt;&gt;"",VLOOKUP(D10,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1237,20 +1273,24 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>106</v>
       </c>
+      <c r="E11" t="str">
+        <f>IFERROR(VLOOKUP(C11,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F11" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A11,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G11),F11,IF(D11&lt;&gt;"",VLOOKUP(D11,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1259,23 +1299,23 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A12,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G12),F12,IF(D12&lt;&gt;"",VLOOKUP(D12,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1284,17 +1324,21 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E13" t="str">
+        <f>IFERROR(VLOOKUP(C13,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F13" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A13,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G13),F13,IF(D13&lt;&gt;"",VLOOKUP(D13,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1303,17 +1347,21 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="E14" t="str">
+        <f>IFERROR(VLOOKUP(C14,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F14" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A14,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G14),F14,IF(D14&lt;&gt;"",VLOOKUP(D14,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1322,17 +1370,21 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="E15" t="str">
+        <f>IFERROR(VLOOKUP(C15,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F15" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A15,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G15),F15,IF(D15&lt;&gt;"",VLOOKUP(D15,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1341,20 +1393,24 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="E16" t="str">
+        <f>IFERROR(VLOOKUP(C16,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F16" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A16,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G16),F16,IF(D16&lt;&gt;"",VLOOKUP(D16,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1363,20 +1419,24 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="E17" t="str">
+        <f>IFERROR(VLOOKUP(C17,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F17" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A17,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G17),F17,IF(D17&lt;&gt;"",VLOOKUP(D17,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1385,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1393,15 +1453,19 @@
       <c r="D18">
         <v>16</v>
       </c>
+      <c r="E18" t="str">
+        <f>IFERROR(VLOOKUP(C18,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F18" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A18,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G18),F18,IF(D18&lt;&gt;"",VLOOKUP(D18,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1410,7 +1474,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1418,15 +1482,19 @@
       <c r="D19">
         <v>17</v>
       </c>
+      <c r="E19" t="str">
+        <f>IFERROR(VLOOKUP(C19,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F19" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A19,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G19),F19,IF(D19&lt;&gt;"",VLOOKUP(D19,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1435,7 +1503,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -1443,18 +1511,19 @@
       <c r="D20">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
-        <v>17</v>
+      <c r="E20" t="str">
+        <f>IFERROR(VLOOKUP(C20,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F20" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A20,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
       </c>
       <c r="H20" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G20),F20,IF(D20&lt;&gt;"",VLOOKUP(D20,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1463,20 +1532,24 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21">
         <v>13</v>
       </c>
+      <c r="E21" t="str">
+        <f>IFERROR(VLOOKUP(C21,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F21" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A21,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G21),F21,IF(D21&lt;&gt;"",VLOOKUP(D21,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1485,20 +1558,24 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22">
         <v>106</v>
       </c>
+      <c r="E22" t="str">
+        <f>IFERROR(VLOOKUP(C22,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F22" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A22,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
       </c>
       <c r="H22" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G22),F22,IF(D22&lt;&gt;"",VLOOKUP(D22,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1507,20 +1584,24 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23">
         <v>21</v>
       </c>
+      <c r="E23" t="str">
+        <f>IFERROR(VLOOKUP(C23,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F23" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A23,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
       </c>
       <c r="H23" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G23),F23,IF(D23&lt;&gt;"",VLOOKUP(D23,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1529,7 +1610,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24">
         <v>21</v>
@@ -1537,15 +1618,19 @@
       <c r="D24">
         <v>22</v>
       </c>
+      <c r="E24" t="str">
+        <f>IFERROR(VLOOKUP(C24,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F24" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A24,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G24),F24,IF(D24&lt;&gt;"",VLOOKUP(D24,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1554,7 +1639,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>21</v>
@@ -1562,15 +1647,19 @@
       <c r="D25">
         <v>23</v>
       </c>
+      <c r="E25" t="str">
+        <f>IFERROR(VLOOKUP(C25,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F25" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A25,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="H25" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G25),F25,IF(D25&lt;&gt;"",VLOOKUP(D25,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1579,7 +1668,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <v>21</v>
@@ -1587,15 +1676,19 @@
       <c r="D26">
         <v>24</v>
       </c>
+      <c r="E26" t="str">
+        <f>IFERROR(VLOOKUP(C26,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F26" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A26,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
       </c>
       <c r="H26" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G26),F26,IF(D26&lt;&gt;"",VLOOKUP(D26,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1604,20 +1697,24 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
+      <c r="E27" t="str">
+        <f>IFERROR(VLOOKUP(C27,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F27" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A27,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
       </c>
       <c r="H27" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G27),F27,IF(D27&lt;&gt;"",VLOOKUP(D27,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1626,7 +1723,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28">
         <v>26</v>
@@ -1634,15 +1731,19 @@
       <c r="D28">
         <v>28</v>
       </c>
+      <c r="E28" t="str">
+        <f>IFERROR(VLOOKUP(C28,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F28" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A28,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
       <c r="H28" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G28),F28,IF(D28&lt;&gt;"",VLOOKUP(D28,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1651,17 +1752,21 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="E29" t="str">
+        <f>IFERROR(VLOOKUP(C29,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F29" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A29,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
       </c>
       <c r="H29" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G29),F29,IF(D29&lt;&gt;"",VLOOKUP(D29,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1670,7 +1775,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>26</v>
@@ -1678,15 +1783,19 @@
       <c r="D30">
         <v>27</v>
       </c>
+      <c r="E30" t="str">
+        <f>IFERROR(VLOOKUP(C30,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F30" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A30,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
       </c>
       <c r="H30" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G30),F30,IF(D30&lt;&gt;"",VLOOKUP(D30,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1695,20 +1804,24 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>105</v>
       </c>
+      <c r="E31" t="str">
+        <f>IFERROR(VLOOKUP(C31,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F31" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A31,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="H31" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G31),F31,IF(D31&lt;&gt;"",VLOOKUP(D31,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>30</v>
@@ -1725,15 +1838,19 @@
       <c r="D32">
         <v>26</v>
       </c>
+      <c r="E32" t="str">
+        <f>IFERROR(VLOOKUP(C32,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F32" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A32,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
       <c r="H32" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G32),F32,IF(D32&lt;&gt;"",VLOOKUP(D32,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1742,7 +1859,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33">
         <v>26</v>
@@ -1750,15 +1867,19 @@
       <c r="D33">
         <v>27</v>
       </c>
+      <c r="E33" t="str">
+        <f>IFERROR(VLOOKUP(C33,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F33" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A33,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
       </c>
       <c r="H33" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G33),F33,IF(D33&lt;&gt;"",VLOOKUP(D33,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1767,7 +1888,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34">
         <v>9</v>
@@ -1775,15 +1896,19 @@
       <c r="D34">
         <v>26</v>
       </c>
+      <c r="E34" t="str">
+        <f>IFERROR(VLOOKUP(C34,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F34" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A34,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G34),F34,IF(D34&lt;&gt;"",VLOOKUP(D34,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1792,20 +1917,24 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
+      <c r="E35" t="str">
+        <f>IFERROR(VLOOKUP(C35,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F35" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A35,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
       </c>
       <c r="H35" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G35),F35,IF(D35&lt;&gt;"",VLOOKUP(D35,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1814,7 +1943,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36">
         <v>105</v>
@@ -1822,15 +1951,19 @@
       <c r="D36">
         <v>9</v>
       </c>
+      <c r="E36" t="str">
+        <f>IFERROR(VLOOKUP(C36,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F36" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A36,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
       <c r="H36" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G36),F36,IF(D36&lt;&gt;"",VLOOKUP(D36,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1839,7 +1972,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>105</v>
@@ -1847,15 +1980,19 @@
       <c r="D37">
         <v>9</v>
       </c>
+      <c r="E37" t="str">
+        <f>IFERROR(VLOOKUP(C37,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F37" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A37,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G37),F37,IF(D37&lt;&gt;"",VLOOKUP(D37,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1864,20 +2001,24 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38">
         <v>105</v>
       </c>
+      <c r="E38" t="str">
+        <f>IFERROR(VLOOKUP(C38,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F38" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A38,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
       <c r="H38" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G38),F38,IF(D38&lt;&gt;"",VLOOKUP(D38,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1886,20 +2027,24 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
+      <c r="E39" t="str">
+        <f>IFERROR(VLOOKUP(C39,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F39" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A39,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
       </c>
       <c r="H39" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G39),F39,IF(D39&lt;&gt;"",VLOOKUP(D39,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -1908,7 +2053,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1916,15 +2061,19 @@
       <c r="D40">
         <v>39</v>
       </c>
+      <c r="E40" t="str">
+        <f>IFERROR(VLOOKUP(C40,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F40" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A40,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
       <c r="H40" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G40),F40,IF(D40&lt;&gt;"",VLOOKUP(D40,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1933,7 +2082,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -1941,15 +2090,19 @@
       <c r="D41">
         <v>5</v>
       </c>
+      <c r="E41" t="str">
+        <f>IFERROR(VLOOKUP(C41,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F41" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A41,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
       <c r="H41" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G41),F41,IF(D41&lt;&gt;"",VLOOKUP(D41,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1958,7 +2111,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -1966,15 +2119,19 @@
       <c r="D42">
         <v>41</v>
       </c>
+      <c r="E42" t="str">
+        <f>IFERROR(VLOOKUP(C42,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F42" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A42,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
       <c r="H42" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G42),F42,IF(D42&lt;&gt;"",VLOOKUP(D42,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -1983,7 +2140,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -1991,15 +2148,19 @@
       <c r="D43">
         <v>42</v>
       </c>
+      <c r="E43" t="str">
+        <f>IFERROR(VLOOKUP(C43,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F43" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A43,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
       <c r="H43" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G43),F43,IF(D43&lt;&gt;"",VLOOKUP(D43,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2008,7 +2169,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -2016,15 +2177,19 @@
       <c r="D44">
         <v>43</v>
       </c>
+      <c r="E44" t="str">
+        <f>IFERROR(VLOOKUP(C44,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F44" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A44,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
       </c>
       <c r="H44" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G44),F44,IF(D44&lt;&gt;"",VLOOKUP(D44,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2033,7 +2198,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -2041,15 +2206,19 @@
       <c r="D45">
         <v>44</v>
       </c>
+      <c r="E45" t="str">
+        <f>IFERROR(VLOOKUP(C45,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F45" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A45,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
       </c>
       <c r="H45" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G45),F45,IF(D45&lt;&gt;"",VLOOKUP(D45,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2058,7 +2227,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -2066,15 +2235,19 @@
       <c r="D46">
         <v>40</v>
       </c>
+      <c r="E46" t="str">
+        <f>IFERROR(VLOOKUP(C46,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F46" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A46,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
       </c>
       <c r="H46" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G46),F46,IF(D46&lt;&gt;"",VLOOKUP(D46,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2083,7 +2256,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -2091,15 +2264,19 @@
       <c r="D47">
         <v>46</v>
       </c>
+      <c r="E47" t="str">
+        <f>IFERROR(VLOOKUP(C47,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F47" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A47,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
       <c r="H47" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G47),F47,IF(D47&lt;&gt;"",VLOOKUP(D47,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2108,20 +2285,24 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48">
         <v>4</v>
       </c>
+      <c r="E48" t="str">
+        <f>IFERROR(VLOOKUP(C48,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F48" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A48,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
       </c>
       <c r="H48" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G48),F48,IF(D48&lt;&gt;"",VLOOKUP(D48,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2130,7 +2311,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -2138,15 +2319,19 @@
       <c r="D49">
         <v>48</v>
       </c>
+      <c r="E49" t="str">
+        <f>IFERROR(VLOOKUP(C49,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F49" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A49,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
       </c>
       <c r="H49" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G49),F49,IF(D49&lt;&gt;"",VLOOKUP(D49,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2155,20 +2340,24 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C50">
         <v>108</v>
       </c>
+      <c r="E50" t="str">
+        <f>IFERROR(VLOOKUP(C50,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F50" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A50,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
       </c>
       <c r="H50" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G50),F50,IF(D50&lt;&gt;"",VLOOKUP(D50,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2177,20 +2366,24 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51">
         <v>108</v>
       </c>
+      <c r="E51" t="str">
+        <f>IFERROR(VLOOKUP(C51,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F51" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A51,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
       </c>
       <c r="H51" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G51),F51,IF(D51&lt;&gt;"",VLOOKUP(D51,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2199,7 +2392,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52">
         <v>108</v>
@@ -2207,15 +2400,19 @@
       <c r="D52">
         <v>51</v>
       </c>
+      <c r="E52" t="str">
+        <f>IFERROR(VLOOKUP(C52,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F52" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A52,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G52),F52,IF(D52&lt;&gt;"",VLOOKUP(D52,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2224,20 +2421,23 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>13</v>
       </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
       <c r="F53" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A53,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
       <c r="H53" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G53),F53,IF(D53&lt;&gt;"",VLOOKUP(D53,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2246,7 +2446,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <v>13</v>
@@ -2254,15 +2454,19 @@
       <c r="D54">
         <v>53</v>
       </c>
+      <c r="E54" t="str">
+        <f>IFERROR(VLOOKUP(C54,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F54" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A54,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
       </c>
       <c r="H54" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G54),F54,IF(D54&lt;&gt;"",VLOOKUP(D54,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2271,7 +2475,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55">
         <v>13</v>
@@ -2279,15 +2483,19 @@
       <c r="D55">
         <v>54</v>
       </c>
+      <c r="E55" t="str">
+        <f>IFERROR(VLOOKUP(C55,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F55" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A55,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
       </c>
       <c r="H55" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G55),F55,IF(D55&lt;&gt;"",VLOOKUP(D55,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2296,7 +2504,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <v>13</v>
@@ -2304,15 +2512,19 @@
       <c r="D56">
         <v>55</v>
       </c>
+      <c r="E56" t="str">
+        <f>IFERROR(VLOOKUP(C56,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F56" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A56,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
       </c>
       <c r="H56" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G56),F56,IF(D56&lt;&gt;"",VLOOKUP(D56,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2321,20 +2533,24 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C57">
         <v>7</v>
       </c>
+      <c r="E57" t="str">
+        <f>IFERROR(VLOOKUP(C57,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F57" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A57,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
       </c>
       <c r="H57" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G57),F57,IF(D57&lt;&gt;"",VLOOKUP(D57,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2343,7 +2559,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -2351,15 +2567,19 @@
       <c r="D58">
         <v>57</v>
       </c>
+      <c r="E58" t="str">
+        <f>IFERROR(VLOOKUP(C58,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F58" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A58,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
       </c>
       <c r="H58" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G58),F58,IF(D58&lt;&gt;"",VLOOKUP(D58,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2368,7 +2588,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C59">
         <v>7</v>
@@ -2376,15 +2596,19 @@
       <c r="D59">
         <v>57</v>
       </c>
+      <c r="E59" t="str">
+        <f>IFERROR(VLOOKUP(C59,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F59" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A59,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
       </c>
       <c r="H59" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G59),F59,IF(D59&lt;&gt;"",VLOOKUP(D59,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2393,7 +2617,7 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60">
         <v>7</v>
@@ -2401,15 +2625,19 @@
       <c r="D60">
         <v>57</v>
       </c>
+      <c r="E60" t="str">
+        <f>IFERROR(VLOOKUP(C60,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F60" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A60,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
       </c>
       <c r="H60" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G60),F60,IF(D60&lt;&gt;"",VLOOKUP(D60,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2418,20 +2646,24 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61">
         <v>7</v>
       </c>
+      <c r="E61" t="str">
+        <f>IFERROR(VLOOKUP(C61,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F61" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A61,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
       </c>
       <c r="H61" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G61),F61,IF(D61&lt;&gt;"",VLOOKUP(D61,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2440,20 +2672,24 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62">
         <v>10</v>
       </c>
+      <c r="E62" t="str">
+        <f>IFERROR(VLOOKUP(C62,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F62" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A62,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
       </c>
       <c r="H62" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G62),F62,IF(D62&lt;&gt;"",VLOOKUP(D62,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2462,68 +2698,83 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>10</v>
       </c>
+      <c r="E63" t="str">
+        <f>IFERROR(VLOOKUP(C63,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F63" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A63,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
       </c>
       <c r="H63" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <f>AND(NOT(G63),F63,IF(D63&lt;&gt;"",VLOOKUP(D63,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64">
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64">
         <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="E64" t="str">
+        <f>IFERROR(VLOOKUP(C64,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F64" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A64,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
       </c>
       <c r="H64" t="e">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G64),F64,IF(D64&lt;&gt;"",VLOOKUP(D64,A$2:G$120,7),TRUE))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" hidden="1">
       <c r="A65">
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65">
         <v>107</v>
       </c>
+      <c r="D65">
+        <v>67</v>
+      </c>
+      <c r="E65" t="str">
+        <f>IFERROR(VLOOKUP(C65,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F65" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A65,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
       </c>
       <c r="H65" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>AND(NOT(G65),F65,IF(D65&lt;&gt;"",VLOOKUP(D65,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8" hidden="1">
@@ -2531,7 +2782,7 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66">
         <v>107</v>
@@ -2539,15 +2790,19 @@
       <c r="D66">
         <v>11</v>
       </c>
+      <c r="E66" t="str">
+        <f>IFERROR(VLOOKUP(C66,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F66" t="b">
-        <f t="shared" si="0"/>
+        <f>ISERROR(MATCH(A66,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
       </c>
       <c r="H66" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(G66),F66,IF(D66&lt;&gt;"",VLOOKUP(D66,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2556,7 +2811,7 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67">
         <v>11</v>
@@ -2564,15 +2819,19 @@
       <c r="D67">
         <v>71</v>
       </c>
+      <c r="E67" t="str">
+        <f>IFERROR(VLOOKUP(C67,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F67" t="b">
-        <f t="shared" ref="F67:F113" si="2">ISERROR(MATCH(A67,C$2:C$113,0))</f>
+        <f>ISERROR(MATCH(A67,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
       <c r="H67" t="b">
-        <f t="shared" ref="H67:H113" si="3">AND(NOT(G67),F67,IF(D67&lt;&gt;"",VLOOKUP(D67,A$2:G$113,7),TRUE))</f>
+        <f>AND(NOT(G67),F67,IF(D67&lt;&gt;"",VLOOKUP(D67,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2581,20 +2840,24 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C68">
         <v>11</v>
       </c>
+      <c r="E68" t="str">
+        <f>IFERROR(VLOOKUP(C68,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F68" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A68,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G68" t="b">
         <v>0</v>
       </c>
       <c r="H68" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G68),F68,IF(D68&lt;&gt;"",VLOOKUP(D68,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2603,23 +2866,23 @@
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>106</v>
       </c>
       <c r="E69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F69" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A69,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
       </c>
       <c r="H69" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G69),F69,IF(D69&lt;&gt;"",VLOOKUP(D69,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2628,20 +2891,24 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C70">
         <v>72</v>
       </c>
+      <c r="E70" t="str">
+        <f>IFERROR(VLOOKUP(C70,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F70" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A70,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
       </c>
       <c r="H70" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G70),F70,IF(D70&lt;&gt;"",VLOOKUP(D70,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2650,45 +2917,53 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71">
         <v>72</v>
       </c>
+      <c r="E71" t="str">
+        <f>IFERROR(VLOOKUP(C71,A$2:G$120,5),"")</f>
+        <v>?</v>
+      </c>
       <c r="F71" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A71,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G71" t="b">
         <v>0</v>
       </c>
       <c r="H71" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <f>AND(NOT(G71),F71,IF(D71&lt;&gt;"",VLOOKUP(D71,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" hidden="1">
       <c r="A72">
         <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72">
         <v>72</v>
       </c>
       <c r="D72" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="E72" t="str">
+        <f>IFERROR(VLOOKUP(C72,A$2:G$120,5),"")</f>
+        <v>?</v>
       </c>
       <c r="F72" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A72,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
       </c>
       <c r="H72" t="e">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G72),F72,IF(D72&lt;&gt;"",VLOOKUP(D72,A$2:G$120,7),TRUE))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2697,7 +2972,7 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73">
         <v>107</v>
@@ -2705,40 +2980,48 @@
       <c r="D73">
         <v>68</v>
       </c>
+      <c r="E73" t="str">
+        <f>IFERROR(VLOOKUP(C73,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F73" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A73,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G73" t="b">
         <v>0</v>
       </c>
       <c r="H73" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <f>AND(NOT(G73),F73,IF(D73&lt;&gt;"",VLOOKUP(D73,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" hidden="1">
       <c r="A74">
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74">
         <v>107</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E74" t="str">
+        <f>IFERROR(VLOOKUP(C74,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F74" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A74,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
       </c>
       <c r="H74" t="e">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G74),F74,IF(D74&lt;&gt;"",VLOOKUP(D74,A$2:G$120,7),TRUE))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2747,7 +3030,7 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C75">
         <v>14</v>
@@ -2755,15 +3038,19 @@
       <c r="D75">
         <v>3</v>
       </c>
+      <c r="E75" t="str">
+        <f>IFERROR(VLOOKUP(C75,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F75" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A75,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
       </c>
       <c r="H75" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G75),F75,IF(D75&lt;&gt;"",VLOOKUP(D75,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2772,20 +3059,24 @@
         <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C76">
         <v>14</v>
       </c>
+      <c r="E76" t="str">
+        <f>IFERROR(VLOOKUP(C76,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F76" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A76,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G76" t="b">
         <v>0</v>
       </c>
       <c r="H76" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G76),F76,IF(D76&lt;&gt;"",VLOOKUP(D76,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2794,20 +3085,24 @@
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C77">
         <v>2</v>
       </c>
+      <c r="E77" t="str">
+        <f>IFERROR(VLOOKUP(C77,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F77" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A77,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
       </c>
       <c r="H77" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G77),F77,IF(D77&lt;&gt;"",VLOOKUP(D77,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2821,15 +3116,19 @@
       <c r="C78">
         <v>102</v>
       </c>
+      <c r="E78" t="str">
+        <f>IFERROR(VLOOKUP(C78,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F78" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A78,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
       </c>
       <c r="H78" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G78),F78,IF(D78&lt;&gt;"",VLOOKUP(D78,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2843,15 +3142,19 @@
       <c r="C79">
         <v>81</v>
       </c>
+      <c r="E79" t="str">
+        <f>IFERROR(VLOOKUP(C79,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F79" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A79,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
       </c>
       <c r="H79" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G79),F79,IF(D79&lt;&gt;"",VLOOKUP(D79,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2865,15 +3168,19 @@
       <c r="C80">
         <v>81</v>
       </c>
+      <c r="E80" t="str">
+        <f>IFERROR(VLOOKUP(C80,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F80" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A80,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G80" t="b">
         <v>0</v>
       </c>
       <c r="H80" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G80),F80,IF(D80&lt;&gt;"",VLOOKUP(D80,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -2887,21 +3194,25 @@
       <c r="C81">
         <v>102</v>
       </c>
+      <c r="E81" t="str">
+        <f>IFERROR(VLOOKUP(C81,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F81" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A81,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G81" t="b">
         <v>0</v>
       </c>
       <c r="H81" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <f>AND(NOT(G81),F81,IF(D81&lt;&gt;"",VLOOKUP(D81,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" hidden="1">
       <c r="A82">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
         <v>14</v>
@@ -2909,37 +3220,48 @@
       <c r="C82">
         <v>102</v>
       </c>
+      <c r="E82" t="str">
+        <f>IFERROR(VLOOKUP(C82,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F82" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ISERROR(MATCH(A82,C$2:C$120,0))</f>
+        <v>0</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
       </c>
       <c r="H82" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>AND(NOT(G82),F82,IF(D82&lt;&gt;"",VLOOKUP(D82,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:8" hidden="1">
       <c r="A83">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
         <v>15</v>
       </c>
       <c r="C83">
-        <v>102</v>
+        <v>86</v>
+      </c>
+      <c r="D83">
+        <v>14</v>
+      </c>
+      <c r="E83" t="str">
+        <f>IFERROR(VLOOKUP(C83,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F83" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>ISERROR(MATCH(A83,C$2:C$120,0))</f>
+        <v>1</v>
       </c>
       <c r="G83" t="b">
         <v>0</v>
       </c>
       <c r="H83" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G83),F83,IF(D83&lt;&gt;"",VLOOKUP(D83,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2948,49 +3270,57 @@
         <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C84">
+        <v>102</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" t="str">
+        <f>IFERROR(VLOOKUP(C84,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F84" t="b">
+        <f>ISERROR(MATCH(A84,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" t="e">
+        <f>AND(NOT(G84),F84,IF(D84&lt;&gt;"",VLOOKUP(D84,A$2:G$120,7),TRUE))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" hidden="1">
+      <c r="A85">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85">
         <v>86</v>
       </c>
-      <c r="D84">
-        <v>14</v>
-      </c>
-      <c r="F84" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G84" t="b">
-        <v>0</v>
-      </c>
-      <c r="H84" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85">
-        <v>87</v>
-      </c>
-      <c r="B85" t="s">
-        <v>22</v>
-      </c>
-      <c r="C85">
-        <v>102</v>
-      </c>
-      <c r="D85" t="s">
-        <v>23</v>
+      <c r="D85">
+        <v>12</v>
+      </c>
+      <c r="E85" t="str">
+        <f>IFERROR(VLOOKUP(C85,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F85" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A85,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
       </c>
-      <c r="H85" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H85" t="b">
+        <f>AND(NOT(G85),F85,IF(D85&lt;&gt;"",VLOOKUP(D85,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8" hidden="1">
@@ -2998,48 +3328,56 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C86">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D86">
-        <v>12</v>
+        <v>94</v>
+      </c>
+      <c r="E86" t="str">
+        <f>IFERROR(VLOOKUP(C86,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F86" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A86,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G86" t="b">
         <v>0</v>
       </c>
       <c r="H86" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G86),F86,IF(D86&lt;&gt;"",VLOOKUP(D86,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8" hidden="1">
       <c r="A87">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C87">
         <v>102</v>
       </c>
       <c r="D87">
-        <v>94</v>
+        <v>7</v>
+      </c>
+      <c r="E87" t="str">
+        <f>IFERROR(VLOOKUP(C87,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F87" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ISERROR(MATCH(A87,C$2:C$120,0))</f>
+        <v>0</v>
       </c>
       <c r="G87" t="b">
         <v>0</v>
       </c>
       <c r="H87" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G87),F87,IF(D87&lt;&gt;"",VLOOKUP(D87,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -3048,29 +3386,33 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C88">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D88">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="E88" t="str">
+        <f>IFERROR(VLOOKUP(C88,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F88" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A88,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G88" t="b">
         <v>0</v>
       </c>
       <c r="H88" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G88),F88,IF(D88&lt;&gt;"",VLOOKUP(D88,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:8" hidden="1">
       <c r="A89">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
         <v>19</v>
@@ -3079,134 +3421,154 @@
         <v>86</v>
       </c>
       <c r="D89">
-        <v>12</v>
+        <v>96</v>
+      </c>
+      <c r="E89" t="s">
+        <v>16</v>
       </c>
       <c r="F89" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>ISERROR(MATCH(A89,C$2:C$120,0))</f>
+        <v>1</v>
       </c>
       <c r="G89" t="b">
         <v>0</v>
       </c>
       <c r="H89" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" hidden="1">
+        <f>AND(NOT(G89),F89,IF(D89&lt;&gt;"",VLOOKUP(D89,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90">
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C90">
-        <v>86</v>
-      </c>
-      <c r="D90">
-        <v>96</v>
-      </c>
-      <c r="E90" t="s">
-        <v>17</v>
+        <v>89</v>
+      </c>
+      <c r="E90" t="str">
+        <f>IFERROR(VLOOKUP(C90,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F90" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A90,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
       </c>
       <c r="H90" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>AND(NOT(G90),F90,IF(D90&lt;&gt;"",VLOOKUP(D90,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C91">
         <v>89</v>
       </c>
+      <c r="E91" t="str">
+        <f>IFERROR(VLOOKUP(C91,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F91" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A91,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
       </c>
       <c r="H91" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <f>AND(NOT(G91),F91,IF(D91&lt;&gt;"",VLOOKUP(D91,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" hidden="1">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C92">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="D92">
+        <v>14</v>
+      </c>
+      <c r="E92" t="str">
+        <f>IFERROR(VLOOKUP(C92,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F92" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A92,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
       </c>
       <c r="H92" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <f>AND(NOT(G92),F92,IF(D92&lt;&gt;"",VLOOKUP(D92,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" hidden="1">
       <c r="A93">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93">
-        <v>86</v>
+        <v>53</v>
+      </c>
+      <c r="D93" t="s">
+        <v>121</v>
+      </c>
+      <c r="E93" t="str">
+        <f>IFERROR(VLOOKUP(C93,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F93" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ISERROR(MATCH(A93,C$2:C$120,0))</f>
+        <v>0</v>
       </c>
       <c r="G93" t="b">
         <v>0</v>
       </c>
-      <c r="H93" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+      <c r="H93" t="e">
+        <f>AND(NOT(G93),F93,IF(D93&lt;&gt;"",VLOOKUP(D93,A$2:G$120,7),TRUE))</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
-      </c>
-      <c r="D94" t="s">
-        <v>122</v>
+        <v>24</v>
+      </c>
+      <c r="C94">
+        <v>102</v>
+      </c>
+      <c r="E94" t="str">
+        <f>IFERROR(VLOOKUP(C94,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F94" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>ISERROR(MATCH(A94,C$2:C$120,0))</f>
+        <v>1</v>
       </c>
       <c r="G94" t="b">
         <v>0</v>
       </c>
-      <c r="H94" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H94" t="b">
+        <f>AND(NOT(G94),F94,IF(D94&lt;&gt;"",VLOOKUP(D94,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3214,26 +3576,30 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C95">
-        <v>102</v>
+        <v>92</v>
+      </c>
+      <c r="E95" t="str">
+        <f>IFERROR(VLOOKUP(C95,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F95" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A95,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G95" t="b">
         <v>0</v>
       </c>
       <c r="H95" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G95),F95,IF(D95&lt;&gt;"",VLOOKUP(D95,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>55</v>
@@ -3241,21 +3607,25 @@
       <c r="C96">
         <v>92</v>
       </c>
+      <c r="E96" t="str">
+        <f>IFERROR(VLOOKUP(C96,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F96" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A96,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G96" t="b">
         <v>0</v>
       </c>
       <c r="H96" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <f>AND(NOT(G96),F96,IF(D96&lt;&gt;"",VLOOKUP(D96,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" hidden="1">
       <c r="A97">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>56</v>
@@ -3263,21 +3633,28 @@
       <c r="C97">
         <v>92</v>
       </c>
+      <c r="D97">
+        <v>94</v>
+      </c>
+      <c r="E97" t="str">
+        <f>IFERROR(VLOOKUP(C97,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F97" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A97,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G97" t="b">
         <v>0</v>
       </c>
       <c r="H97" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>AND(NOT(G97),F97,IF(D97&lt;&gt;"",VLOOKUP(D97,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" hidden="1">
       <c r="A98">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>57</v>
@@ -3286,48 +3663,53 @@
         <v>92</v>
       </c>
       <c r="D98">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="E98" t="str">
+        <f>IFERROR(VLOOKUP(C98,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F98" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A98,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
       </c>
       <c r="H98" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" hidden="1">
+        <f>AND(NOT(G98),F98,IF(D98&lt;&gt;"",VLOOKUP(D98,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C99">
-        <v>92</v>
-      </c>
-      <c r="D99">
-        <v>95</v>
+        <v>37</v>
+      </c>
+      <c r="E99" t="str">
+        <f>IFERROR(VLOOKUP(C99,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F99" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A99,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G99" t="b">
         <v>0</v>
       </c>
       <c r="H99" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>AND(NOT(G99),F99,IF(D99&lt;&gt;"",VLOOKUP(D99,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>35</v>
@@ -3335,59 +3717,71 @@
       <c r="C100">
         <v>37</v>
       </c>
+      <c r="E100" t="str">
+        <f>IFERROR(VLOOKUP(C100,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F100" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A100,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G100" t="b">
         <v>0</v>
       </c>
       <c r="H100" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G100),F100,IF(D100&lt;&gt;"",VLOOKUP(D100,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101">
         <v>36</v>
       </c>
-      <c r="C101">
-        <v>37</v>
+      <c r="E101" t="str">
+        <f>IFERROR(VLOOKUP(C101,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F101" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A101,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
       </c>
       <c r="H101" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G101),F101,IF(D101&lt;&gt;"",VLOOKUP(D101,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C102">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="E102" t="str">
+        <f>IFERROR(VLOOKUP(C102,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F102" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A102,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G102" t="b">
         <v>0</v>
       </c>
       <c r="H102" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G102),F102,IF(D102&lt;&gt;"",VLOOKUP(D102,A$2:G$120,7),TRUE))</f>
         <v>1</v>
       </c>
     </row>
@@ -3396,26 +3790,30 @@
         <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C103">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="E103" t="str">
+        <f>IFERROR(VLOOKUP(C103,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F103" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A103,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G103" t="b">
         <v>0</v>
       </c>
       <c r="H103" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <f>AND(NOT(G103),F103,IF(D103&lt;&gt;"",VLOOKUP(D103,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
@@ -3423,219 +3821,437 @@
       <c r="C104">
         <v>33</v>
       </c>
+      <c r="D104">
+        <v>100</v>
+      </c>
+      <c r="E104" t="str">
+        <f>IFERROR(VLOOKUP(C104,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
       <c r="F104" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A104,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G104" t="b">
         <v>0</v>
       </c>
       <c r="H104" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" hidden="1">
+        <f>AND(NOT(G104),F104,IF(D104&lt;&gt;"",VLOOKUP(D104,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105">
         <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C105">
-        <v>33</v>
-      </c>
-      <c r="D105">
-        <v>100</v>
+        <v>35</v>
+      </c>
+      <c r="E105" t="str">
+        <f>IFERROR(VLOOKUP(C105,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F105" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A105,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G105" t="b">
         <v>0</v>
       </c>
       <c r="H105" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+        <f>AND(NOT(G105),F105,IF(D105&lt;&gt;"",VLOOKUP(D105,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" hidden="1">
       <c r="A106">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
-      </c>
-      <c r="C106">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="E106" t="str">
+        <f>IFERROR(VLOOKUP(C106,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F106" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ISERROR(MATCH(A106,C$2:C$120,0))</f>
+        <v>0</v>
       </c>
       <c r="G106" t="b">
         <v>0</v>
       </c>
       <c r="H106" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" hidden="1">
+        <f>AND(NOT(G106),F106,IF(D106&lt;&gt;"",VLOOKUP(D106,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107">
+        <v>103</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107">
         <v>102</v>
       </c>
-      <c r="B107" t="s">
-        <v>4</v>
+      <c r="E107" t="str">
+        <f>IFERROR(VLOOKUP(C107,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F107" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>ISERROR(MATCH(A107,C$2:C$120,0))</f>
+        <v>1</v>
       </c>
       <c r="G107" t="b">
         <v>0</v>
       </c>
       <c r="H107" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <f>AND(NOT(G107),F107,IF(D107&lt;&gt;"",VLOOKUP(D107,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" hidden="1">
       <c r="A108">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108">
+        <v>8</v>
+      </c>
+      <c r="D108">
         <v>7</v>
       </c>
-      <c r="C108">
-        <v>102</v>
+      <c r="E108" t="str">
+        <f>IFERROR(VLOOKUP(C108,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F108" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A108,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G108" t="b">
         <v>0</v>
       </c>
       <c r="H108" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>AND(NOT(G108),F108,IF(D108&lt;&gt;"",VLOOKUP(D108,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8" hidden="1">
       <c r="A109">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
-      </c>
-      <c r="C109">
-        <v>8</v>
-      </c>
-      <c r="D109">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="E109" t="str">
+        <f>IFERROR(VLOOKUP(C109,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F109" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ISERROR(MATCH(A109,C$2:C$120,0))</f>
+        <v>0</v>
       </c>
       <c r="G109" t="b">
         <v>0</v>
       </c>
       <c r="H109" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G109),F109,IF(D109&lt;&gt;"",VLOOKUP(D109,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" hidden="1">
       <c r="A110">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>26</v>
+        <v>65</v>
+      </c>
+      <c r="E110" t="str">
+        <f>IFERROR(VLOOKUP(C110,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F110" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A110,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G110" t="b">
         <v>0</v>
       </c>
       <c r="H110" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G110),F110,IF(D110&lt;&gt;"",VLOOKUP(D110,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:8" hidden="1">
       <c r="A111">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
+        <v>85</v>
+      </c>
+      <c r="E111" t="str">
+        <f>IFERROR(VLOOKUP(C111,A$2:G$120,5),"")</f>
+        <v/>
       </c>
       <c r="F111" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A111,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
       </c>
       <c r="H111" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G111),F111,IF(D111&lt;&gt;"",VLOOKUP(D111,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:8" hidden="1">
       <c r="A112">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
-        <v>86</v>
+        <v>105</v>
+      </c>
+      <c r="C112">
+        <v>13</v>
+      </c>
+      <c r="E112" t="s">
+        <v>16</v>
       </c>
       <c r="F112" t="b">
-        <f t="shared" si="2"/>
+        <f>ISERROR(MATCH(A112,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G112" t="b">
         <v>0</v>
       </c>
       <c r="H112" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(G112),F112,IF(D112&lt;&gt;"",VLOOKUP(D112,A$2:G$120,7),TRUE))</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:8" hidden="1">
       <c r="A113">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B113" t="s">
+        <v>125</v>
+      </c>
+      <c r="C113">
+        <v>102</v>
+      </c>
+      <c r="E113" t="str">
+        <f>IFERROR(VLOOKUP(C113,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F113" t="b">
+        <f>ISERROR(MATCH(A113,C$2:C$120,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" t="b">
+        <f>AND(NOT(G113),F113,IF(D113&lt;&gt;"",VLOOKUP(D113,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114">
+        <v>110</v>
+      </c>
+      <c r="B114" t="s">
+        <v>126</v>
+      </c>
+      <c r="C114">
+        <v>109</v>
+      </c>
+      <c r="E114" t="str">
+        <f>IFERROR(VLOOKUP(C114,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F114" t="b">
+        <f>ISERROR(MATCH(A114,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" t="b">
+        <f>AND(NOT(G114),F114,IF(D114&lt;&gt;"",VLOOKUP(D114,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115">
+        <v>111</v>
+      </c>
+      <c r="B115" t="s">
+        <v>127</v>
+      </c>
+      <c r="C115">
+        <v>109</v>
+      </c>
+      <c r="E115" t="str">
+        <f>IFERROR(VLOOKUP(C115,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F115" t="b">
+        <f>ISERROR(MATCH(A115,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" t="b">
+        <f>AND(NOT(G115),F115,IF(D115&lt;&gt;"",VLOOKUP(D115,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116">
+        <v>112</v>
+      </c>
+      <c r="B116" t="s">
+        <v>128</v>
+      </c>
+      <c r="C116">
+        <v>109</v>
+      </c>
+      <c r="E116" t="str">
+        <f>IFERROR(VLOOKUP(C116,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F116" t="b">
+        <f>ISERROR(MATCH(A116,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" t="b">
+        <f>AND(NOT(G116),F116,IF(D116&lt;&gt;"",VLOOKUP(D116,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117">
+        <v>113</v>
+      </c>
+      <c r="B117" t="s">
+        <v>129</v>
+      </c>
+      <c r="C117">
+        <v>109</v>
+      </c>
+      <c r="E117" t="str">
+        <f>IFERROR(VLOOKUP(C117,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F117" t="b">
+        <f>ISERROR(MATCH(A117,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" t="b">
+        <f>AND(NOT(G117),F117,IF(D117&lt;&gt;"",VLOOKUP(D117,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" hidden="1">
+      <c r="A118">
+        <v>114</v>
+      </c>
+      <c r="B118" t="s">
+        <v>130</v>
+      </c>
+      <c r="C118">
+        <v>107</v>
+      </c>
+      <c r="D118">
+        <v>68</v>
+      </c>
+      <c r="E118" t="str">
+        <f>IFERROR(VLOOKUP(C118,A$2:G$120,5),"")</f>
+        <v/>
+      </c>
+      <c r="F118" t="b">
+        <f>ISERROR(MATCH(A118,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" t="b">
+        <f>AND(NOT(G118),F118,IF(D118&lt;&gt;"",VLOOKUP(D118,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119">
+        <v>115</v>
+      </c>
+      <c r="B119" t="s">
+        <v>131</v>
+      </c>
+      <c r="C119">
         <v>106</v>
       </c>
-      <c r="C113">
-        <v>13</v>
-      </c>
-      <c r="E113" t="s">
-        <v>17</v>
-      </c>
-      <c r="F113" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G113" t="b">
-        <v>0</v>
-      </c>
-      <c r="H113" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="E119" t="s">
+        <v>16</v>
+      </c>
+      <c r="F119" t="b">
+        <f>ISERROR(MATCH(A119,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119" t="b">
+        <f>AND(NOT(G119),F119,IF(D119&lt;&gt;"",VLOOKUP(D119,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120">
+        <v>116</v>
+      </c>
+      <c r="B120" t="s">
+        <v>132</v>
+      </c>
+      <c r="C120">
+        <v>106</v>
+      </c>
+      <c r="E120" t="s">
+        <v>16</v>
+      </c>
+      <c r="F120" t="b">
+        <f>ISERROR(MATCH(A120,C$2:C$120,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" t="b">
+        <f>AND(NOT(G120),F120,IF(D120&lt;&gt;"",VLOOKUP(D120,A$2:G$120,7),TRUE))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H113">
+  <autoFilter ref="A1:H120">
     <filterColumn colId="7">
       <filters>
         <filter val="TRUE"/>
-        <filter val="#N/A"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Fixed joint angles in state server RAPID.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="19440" windowHeight="12075"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$120</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -423,8 +423,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,217 +459,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -776,6 +566,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -810,6 +601,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -985,24 +777,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="585" activePane="bottomLeft"/>
+      <pane ySplit="585" topLeftCell="A79" activePane="bottomLeft"/>
       <selection activeCell="A60" sqref="A60"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="78.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +819,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1039,22 +830,22 @@
         <v>14</v>
       </c>
       <c r="E2" t="str">
-        <f>IFERROR(VLOOKUP(C2,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E2:E11" si="0">IFERROR(VLOOKUP(C2,A$2:G$120,5),"")</f>
         <v/>
       </c>
       <c r="F2" t="b">
-        <f>ISERROR(MATCH(A2,C$2:C$120,0))</f>
+        <f t="shared" ref="F2:F33" si="1">ISERROR(MATCH(A2,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <f>AND(NOT(G2),F2,IF(D2&lt;&gt;"",VLOOKUP(D2,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" hidden="1">
+        <f t="shared" ref="H2:H33" si="2">AND(NOT(G2),F2,IF(D2&lt;&gt;"",VLOOKUP(D2,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1065,22 +856,22 @@
         <v>14</v>
       </c>
       <c r="E3" t="str">
-        <f>IFERROR(VLOOKUP(C3,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F3" t="b">
-        <f>ISERROR(MATCH(A3,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <f>AND(NOT(G3),F3,IF(D3&lt;&gt;"",VLOOKUP(D3,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1094,22 +885,22 @@
         <v>68</v>
       </c>
       <c r="E4" t="str">
-        <f>IFERROR(VLOOKUP(C4,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F4" t="b">
-        <f>ISERROR(MATCH(A4,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <f>AND(NOT(G4),F4,IF(D4&lt;&gt;"",VLOOKUP(D4,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1120,22 +911,22 @@
         <v>13</v>
       </c>
       <c r="E5" t="str">
-        <f>IFERROR(VLOOKUP(C5,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F5" t="b">
-        <f>ISERROR(MATCH(A5,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <f>AND(NOT(G5),F5,IF(D5&lt;&gt;"",VLOOKUP(D5,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1146,22 +937,22 @@
         <v>13</v>
       </c>
       <c r="E6" t="str">
-        <f>IFERROR(VLOOKUP(C6,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F6" t="b">
-        <f>ISERROR(MATCH(A6,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="H6" t="b">
-        <f>AND(NOT(G6),F6,IF(D6&lt;&gt;"",VLOOKUP(D6,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1172,22 +963,22 @@
         <v>13</v>
       </c>
       <c r="E7" t="str">
-        <f>IFERROR(VLOOKUP(C7,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F7" t="b">
-        <f>ISERROR(MATCH(A7,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
       <c r="H7" t="b">
-        <f>AND(NOT(G7),F7,IF(D7&lt;&gt;"",VLOOKUP(D7,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1198,22 +989,22 @@
         <v>12</v>
       </c>
       <c r="E8" t="str">
-        <f>IFERROR(VLOOKUP(C8,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F8" t="b">
-        <f>ISERROR(MATCH(A8,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="H8" t="b">
-        <f>AND(NOT(G8),F8,IF(D8&lt;&gt;"",VLOOKUP(D8,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1227,22 +1018,22 @@
         <v>120</v>
       </c>
       <c r="E9" t="str">
-        <f>IFERROR(VLOOKUP(C9,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F9" t="b">
-        <f>ISERROR(MATCH(A9,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="e">
-        <f>AND(NOT(G9),F9,IF(D9&lt;&gt;"",VLOOKUP(D9,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1253,22 +1044,22 @@
         <v>12</v>
       </c>
       <c r="E10" t="str">
-        <f>IFERROR(VLOOKUP(C10,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F10" t="b">
-        <f>ISERROR(MATCH(A10,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <f>AND(NOT(G10),F10,IF(D10&lt;&gt;"",VLOOKUP(D10,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1279,22 +1070,22 @@
         <v>106</v>
       </c>
       <c r="E11" t="str">
-        <f>IFERROR(VLOOKUP(C11,A$2:G$120,5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F11" t="b">
-        <f>ISERROR(MATCH(A11,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="b">
-        <f>AND(NOT(G11),F11,IF(D11&lt;&gt;"",VLOOKUP(D11,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1308,18 +1099,18 @@
         <v>16</v>
       </c>
       <c r="F12" t="b">
-        <f>ISERROR(MATCH(A12,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="b">
-        <f>AND(NOT(G12),F12,IF(D12&lt;&gt;"",VLOOKUP(D12,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1327,22 +1118,22 @@
         <v>36</v>
       </c>
       <c r="E13" t="str">
-        <f>IFERROR(VLOOKUP(C13,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E13:E52" si="3">IFERROR(VLOOKUP(C13,A$2:G$120,5),"")</f>
         <v/>
       </c>
       <c r="F13" t="b">
-        <f>ISERROR(MATCH(A13,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <f>AND(NOT(G13),F13,IF(D13&lt;&gt;"",VLOOKUP(D13,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1350,22 +1141,22 @@
         <v>62</v>
       </c>
       <c r="E14" t="str">
-        <f>IFERROR(VLOOKUP(C14,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F14" t="b">
-        <f>ISERROR(MATCH(A14,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="b">
-        <f>AND(NOT(G14),F14,IF(D14&lt;&gt;"",VLOOKUP(D14,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1373,22 +1164,22 @@
         <v>109</v>
       </c>
       <c r="E15" t="str">
-        <f>IFERROR(VLOOKUP(C15,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F15" t="b">
-        <f>ISERROR(MATCH(A15,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="b">
-        <f>AND(NOT(G15),F15,IF(D15&lt;&gt;"",VLOOKUP(D15,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1399,22 +1190,22 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f>IFERROR(VLOOKUP(C16,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F16" t="b">
-        <f>ISERROR(MATCH(A16,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="b">
-        <f>AND(NOT(G16),F16,IF(D16&lt;&gt;"",VLOOKUP(D16,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1425,22 +1216,22 @@
         <v>1</v>
       </c>
       <c r="E17" t="str">
-        <f>IFERROR(VLOOKUP(C17,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F17" t="b">
-        <f>ISERROR(MATCH(A17,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="b">
-        <f>AND(NOT(G17),F17,IF(D17&lt;&gt;"",VLOOKUP(D17,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1454,22 +1245,22 @@
         <v>16</v>
       </c>
       <c r="E18" t="str">
-        <f>IFERROR(VLOOKUP(C18,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F18" t="b">
-        <f>ISERROR(MATCH(A18,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="b">
-        <f>AND(NOT(G18),F18,IF(D18&lt;&gt;"",VLOOKUP(D18,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1483,22 +1274,22 @@
         <v>17</v>
       </c>
       <c r="E19" t="str">
-        <f>IFERROR(VLOOKUP(C19,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F19" t="b">
-        <f>ISERROR(MATCH(A19,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="b">
-        <f>AND(NOT(G19),F19,IF(D19&lt;&gt;"",VLOOKUP(D19,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1512,22 +1303,22 @@
         <v>20</v>
       </c>
       <c r="E20" t="str">
-        <f>IFERROR(VLOOKUP(C20,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F20" t="b">
-        <f>ISERROR(MATCH(A20,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
       </c>
       <c r="H20" t="b">
-        <f>AND(NOT(G20),F20,IF(D20&lt;&gt;"",VLOOKUP(D20,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1538,22 +1329,22 @@
         <v>13</v>
       </c>
       <c r="E21" t="str">
-        <f>IFERROR(VLOOKUP(C21,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F21" t="b">
-        <f>ISERROR(MATCH(A21,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="b">
-        <f>AND(NOT(G21),F21,IF(D21&lt;&gt;"",VLOOKUP(D21,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1564,22 +1355,22 @@
         <v>106</v>
       </c>
       <c r="E22" t="str">
-        <f>IFERROR(VLOOKUP(C22,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F22" t="b">
-        <f>ISERROR(MATCH(A22,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
       </c>
       <c r="H22" t="b">
-        <f>AND(NOT(G22),F22,IF(D22&lt;&gt;"",VLOOKUP(D22,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1590,22 +1381,22 @@
         <v>21</v>
       </c>
       <c r="E23" t="str">
-        <f>IFERROR(VLOOKUP(C23,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F23" t="b">
-        <f>ISERROR(MATCH(A23,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
       </c>
       <c r="H23" t="b">
-        <f>AND(NOT(G23),F23,IF(D23&lt;&gt;"",VLOOKUP(D23,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1619,22 +1410,22 @@
         <v>22</v>
       </c>
       <c r="E24" t="str">
-        <f>IFERROR(VLOOKUP(C24,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F24" t="b">
-        <f>ISERROR(MATCH(A24,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="b">
-        <f>AND(NOT(G24),F24,IF(D24&lt;&gt;"",VLOOKUP(D24,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1648,22 +1439,22 @@
         <v>23</v>
       </c>
       <c r="E25" t="str">
-        <f>IFERROR(VLOOKUP(C25,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F25" t="b">
-        <f>ISERROR(MATCH(A25,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="H25" t="b">
-        <f>AND(NOT(G25),F25,IF(D25&lt;&gt;"",VLOOKUP(D25,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1677,22 +1468,22 @@
         <v>24</v>
       </c>
       <c r="E26" t="str">
-        <f>IFERROR(VLOOKUP(C26,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F26" t="b">
-        <f>ISERROR(MATCH(A26,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
       </c>
       <c r="H26" t="b">
-        <f>AND(NOT(G26),F26,IF(D26&lt;&gt;"",VLOOKUP(D26,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1703,22 +1494,22 @@
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f>IFERROR(VLOOKUP(C27,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F27" t="b">
-        <f>ISERROR(MATCH(A27,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
       </c>
       <c r="H27" t="b">
-        <f>AND(NOT(G27),F27,IF(D27&lt;&gt;"",VLOOKUP(D27,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1732,22 +1523,22 @@
         <v>28</v>
       </c>
       <c r="E28" t="str">
-        <f>IFERROR(VLOOKUP(C28,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F28" t="b">
-        <f>ISERROR(MATCH(A28,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
       <c r="H28" t="b">
-        <f>AND(NOT(G28),F28,IF(D28&lt;&gt;"",VLOOKUP(D28,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1755,22 +1546,22 @@
         <v>84</v>
       </c>
       <c r="E29" t="str">
-        <f>IFERROR(VLOOKUP(C29,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F29" t="b">
-        <f>ISERROR(MATCH(A29,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
       </c>
       <c r="H29" t="b">
-        <f>AND(NOT(G29),F29,IF(D29&lt;&gt;"",VLOOKUP(D29,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1784,22 +1575,22 @@
         <v>27</v>
       </c>
       <c r="E30" t="str">
-        <f>IFERROR(VLOOKUP(C30,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F30" t="b">
-        <f>ISERROR(MATCH(A30,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
       </c>
       <c r="H30" t="b">
-        <f>AND(NOT(G30),F30,IF(D30&lt;&gt;"",VLOOKUP(D30,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1810,22 +1601,22 @@
         <v>105</v>
       </c>
       <c r="E31" t="str">
-        <f>IFERROR(VLOOKUP(C31,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F31" t="b">
-        <f>ISERROR(MATCH(A31,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="H31" t="b">
-        <f>AND(NOT(G31),F31,IF(D31&lt;&gt;"",VLOOKUP(D31,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1839,22 +1630,22 @@
         <v>26</v>
       </c>
       <c r="E32" t="str">
-        <f>IFERROR(VLOOKUP(C32,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F32" t="b">
-        <f>ISERROR(MATCH(A32,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
       <c r="H32" t="b">
-        <f>AND(NOT(G32),F32,IF(D32&lt;&gt;"",VLOOKUP(D32,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1868,22 +1659,22 @@
         <v>27</v>
       </c>
       <c r="E33" t="str">
-        <f>IFERROR(VLOOKUP(C33,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F33" t="b">
-        <f>ISERROR(MATCH(A33,C$2:C$120,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
       </c>
       <c r="H33" t="b">
-        <f>AND(NOT(G33),F33,IF(D33&lt;&gt;"",VLOOKUP(D33,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" hidden="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1897,22 +1688,22 @@
         <v>26</v>
       </c>
       <c r="E34" t="str">
-        <f>IFERROR(VLOOKUP(C34,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F34" t="b">
-        <f>ISERROR(MATCH(A34,C$2:C$120,0))</f>
+        <f t="shared" ref="F34:F65" si="4">ISERROR(MATCH(A34,C$2:C$120,0))</f>
         <v>0</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="b">
-        <f>AND(NOT(G34),F34,IF(D34&lt;&gt;"",VLOOKUP(D34,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <f t="shared" ref="H34:H65" si="5">AND(NOT(G34),F34,IF(D34&lt;&gt;"",VLOOKUP(D34,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1923,22 +1714,22 @@
         <v>33</v>
       </c>
       <c r="E35" t="str">
-        <f>IFERROR(VLOOKUP(C35,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F35" t="b">
-        <f>ISERROR(MATCH(A35,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
       </c>
       <c r="H35" t="b">
-        <f>AND(NOT(G35),F35,IF(D35&lt;&gt;"",VLOOKUP(D35,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1952,22 +1743,22 @@
         <v>9</v>
       </c>
       <c r="E36" t="str">
-        <f>IFERROR(VLOOKUP(C36,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F36" t="b">
-        <f>ISERROR(MATCH(A36,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
       <c r="H36" t="b">
-        <f>AND(NOT(G36),F36,IF(D36&lt;&gt;"",VLOOKUP(D36,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1981,22 +1772,22 @@
         <v>9</v>
       </c>
       <c r="E37" t="str">
-        <f>IFERROR(VLOOKUP(C37,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F37" t="b">
-        <f>ISERROR(MATCH(A37,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" t="b">
-        <f>AND(NOT(G37),F37,IF(D37&lt;&gt;"",VLOOKUP(D37,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2007,22 +1798,22 @@
         <v>105</v>
       </c>
       <c r="E38" t="str">
-        <f>IFERROR(VLOOKUP(C38,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F38" t="b">
-        <f>ISERROR(MATCH(A38,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
       <c r="H38" t="b">
-        <f>AND(NOT(G38),F38,IF(D38&lt;&gt;"",VLOOKUP(D38,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2033,22 +1824,22 @@
         <v>5</v>
       </c>
       <c r="E39" t="str">
-        <f>IFERROR(VLOOKUP(C39,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F39" t="b">
-        <f>ISERROR(MATCH(A39,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
       </c>
       <c r="H39" t="b">
-        <f>AND(NOT(G39),F39,IF(D39&lt;&gt;"",VLOOKUP(D39,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2062,22 +1853,22 @@
         <v>39</v>
       </c>
       <c r="E40" t="str">
-        <f>IFERROR(VLOOKUP(C40,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F40" t="b">
-        <f>ISERROR(MATCH(A40,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
       <c r="H40" t="b">
-        <f>AND(NOT(G40),F40,IF(D40&lt;&gt;"",VLOOKUP(D40,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2091,22 +1882,22 @@
         <v>5</v>
       </c>
       <c r="E41" t="str">
-        <f>IFERROR(VLOOKUP(C41,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F41" t="b">
-        <f>ISERROR(MATCH(A41,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
       <c r="H41" t="b">
-        <f>AND(NOT(G41),F41,IF(D41&lt;&gt;"",VLOOKUP(D41,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2120,22 +1911,22 @@
         <v>41</v>
       </c>
       <c r="E42" t="str">
-        <f>IFERROR(VLOOKUP(C42,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F42" t="b">
-        <f>ISERROR(MATCH(A42,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
       <c r="H42" t="b">
-        <f>AND(NOT(G42),F42,IF(D42&lt;&gt;"",VLOOKUP(D42,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2149,22 +1940,22 @@
         <v>42</v>
       </c>
       <c r="E43" t="str">
-        <f>IFERROR(VLOOKUP(C43,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F43" t="b">
-        <f>ISERROR(MATCH(A43,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
       <c r="H43" t="b">
-        <f>AND(NOT(G43),F43,IF(D43&lt;&gt;"",VLOOKUP(D43,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2178,22 +1969,22 @@
         <v>43</v>
       </c>
       <c r="E44" t="str">
-        <f>IFERROR(VLOOKUP(C44,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F44" t="b">
-        <f>ISERROR(MATCH(A44,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
       </c>
       <c r="H44" t="b">
-        <f>AND(NOT(G44),F44,IF(D44&lt;&gt;"",VLOOKUP(D44,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2207,22 +1998,22 @@
         <v>44</v>
       </c>
       <c r="E45" t="str">
-        <f>IFERROR(VLOOKUP(C45,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F45" t="b">
-        <f>ISERROR(MATCH(A45,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
       </c>
       <c r="H45" t="b">
-        <f>AND(NOT(G45),F45,IF(D45&lt;&gt;"",VLOOKUP(D45,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2236,22 +2027,22 @@
         <v>40</v>
       </c>
       <c r="E46" t="str">
-        <f>IFERROR(VLOOKUP(C46,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F46" t="b">
-        <f>ISERROR(MATCH(A46,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
       </c>
       <c r="H46" t="b">
-        <f>AND(NOT(G46),F46,IF(D46&lt;&gt;"",VLOOKUP(D46,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2265,22 +2056,22 @@
         <v>46</v>
       </c>
       <c r="E47" t="str">
-        <f>IFERROR(VLOOKUP(C47,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F47" t="b">
-        <f>ISERROR(MATCH(A47,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
       <c r="H47" t="b">
-        <f>AND(NOT(G47),F47,IF(D47&lt;&gt;"",VLOOKUP(D47,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2291,22 +2082,22 @@
         <v>4</v>
       </c>
       <c r="E48" t="str">
-        <f>IFERROR(VLOOKUP(C48,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F48" t="b">
-        <f>ISERROR(MATCH(A48,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
       </c>
       <c r="H48" t="b">
-        <f>AND(NOT(G48),F48,IF(D48&lt;&gt;"",VLOOKUP(D48,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2320,22 +2111,22 @@
         <v>48</v>
       </c>
       <c r="E49" t="str">
-        <f>IFERROR(VLOOKUP(C49,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F49" t="b">
-        <f>ISERROR(MATCH(A49,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
       </c>
       <c r="H49" t="b">
-        <f>AND(NOT(G49),F49,IF(D49&lt;&gt;"",VLOOKUP(D49,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2346,22 +2137,22 @@
         <v>108</v>
       </c>
       <c r="E50" t="str">
-        <f>IFERROR(VLOOKUP(C50,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v>?</v>
       </c>
       <c r="F50" t="b">
-        <f>ISERROR(MATCH(A50,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
       </c>
       <c r="H50" t="b">
-        <f>AND(NOT(G50),F50,IF(D50&lt;&gt;"",VLOOKUP(D50,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2372,22 +2163,22 @@
         <v>108</v>
       </c>
       <c r="E51" t="str">
-        <f>IFERROR(VLOOKUP(C51,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v>?</v>
       </c>
       <c r="F51" t="b">
-        <f>ISERROR(MATCH(A51,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
       </c>
       <c r="H51" t="b">
-        <f>AND(NOT(G51),F51,IF(D51&lt;&gt;"",VLOOKUP(D51,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2401,22 +2192,22 @@
         <v>51</v>
       </c>
       <c r="E52" t="str">
-        <f>IFERROR(VLOOKUP(C52,A$2:G$120,5),"")</f>
+        <f t="shared" si="3"/>
         <v>?</v>
       </c>
       <c r="F52" t="b">
-        <f>ISERROR(MATCH(A52,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <f>AND(NOT(G52),F52,IF(D52&lt;&gt;"",VLOOKUP(D52,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2430,18 +2221,18 @@
         <v>16</v>
       </c>
       <c r="F53" t="b">
-        <f>ISERROR(MATCH(A53,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
       <c r="H53" t="b">
-        <f>AND(NOT(G53),F53,IF(D53&lt;&gt;"",VLOOKUP(D53,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2455,22 +2246,22 @@
         <v>53</v>
       </c>
       <c r="E54" t="str">
-        <f>IFERROR(VLOOKUP(C54,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E54:E68" si="6">IFERROR(VLOOKUP(C54,A$2:G$120,5),"")</f>
         <v/>
       </c>
       <c r="F54" t="b">
-        <f>ISERROR(MATCH(A54,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
       </c>
       <c r="H54" t="b">
-        <f>AND(NOT(G54),F54,IF(D54&lt;&gt;"",VLOOKUP(D54,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2484,22 +2275,22 @@
         <v>54</v>
       </c>
       <c r="E55" t="str">
-        <f>IFERROR(VLOOKUP(C55,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F55" t="b">
-        <f>ISERROR(MATCH(A55,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
       </c>
       <c r="H55" t="b">
-        <f>AND(NOT(G55),F55,IF(D55&lt;&gt;"",VLOOKUP(D55,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2513,22 +2304,22 @@
         <v>55</v>
       </c>
       <c r="E56" t="str">
-        <f>IFERROR(VLOOKUP(C56,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F56" t="b">
-        <f>ISERROR(MATCH(A56,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
       </c>
       <c r="H56" t="b">
-        <f>AND(NOT(G56),F56,IF(D56&lt;&gt;"",VLOOKUP(D56,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -2539,22 +2330,22 @@
         <v>7</v>
       </c>
       <c r="E57" t="str">
-        <f>IFERROR(VLOOKUP(C57,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F57" t="b">
-        <f>ISERROR(MATCH(A57,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
       </c>
       <c r="H57" t="b">
-        <f>AND(NOT(G57),F57,IF(D57&lt;&gt;"",VLOOKUP(D57,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -2568,22 +2359,22 @@
         <v>57</v>
       </c>
       <c r="E58" t="str">
-        <f>IFERROR(VLOOKUP(C58,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F58" t="b">
-        <f>ISERROR(MATCH(A58,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
       </c>
       <c r="H58" t="b">
-        <f>AND(NOT(G58),F58,IF(D58&lt;&gt;"",VLOOKUP(D58,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
@@ -2597,22 +2388,22 @@
         <v>57</v>
       </c>
       <c r="E59" t="str">
-        <f>IFERROR(VLOOKUP(C59,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F59" t="b">
-        <f>ISERROR(MATCH(A59,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
       </c>
       <c r="H59" t="b">
-        <f>AND(NOT(G59),F59,IF(D59&lt;&gt;"",VLOOKUP(D59,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>63</v>
       </c>
@@ -2626,22 +2417,22 @@
         <v>57</v>
       </c>
       <c r="E60" t="str">
-        <f>IFERROR(VLOOKUP(C60,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F60" t="b">
-        <f>ISERROR(MATCH(A60,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
       </c>
       <c r="H60" t="b">
-        <f>AND(NOT(G60),F60,IF(D60&lt;&gt;"",VLOOKUP(D60,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>64</v>
       </c>
@@ -2652,22 +2443,22 @@
         <v>7</v>
       </c>
       <c r="E61" t="str">
-        <f>IFERROR(VLOOKUP(C61,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F61" t="b">
-        <f>ISERROR(MATCH(A61,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="b">
-        <f>AND(NOT(G61),F61,IF(D61&lt;&gt;"",VLOOKUP(D61,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>65</v>
       </c>
@@ -2678,22 +2469,22 @@
         <v>10</v>
       </c>
       <c r="E62" t="str">
-        <f>IFERROR(VLOOKUP(C62,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F62" t="b">
-        <f>ISERROR(MATCH(A62,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
       </c>
       <c r="H62" t="b">
-        <f>AND(NOT(G62),F62,IF(D62&lt;&gt;"",VLOOKUP(D62,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>66</v>
       </c>
@@ -2704,22 +2495,22 @@
         <v>10</v>
       </c>
       <c r="E63" t="str">
-        <f>IFERROR(VLOOKUP(C63,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F63" t="b">
-        <f>ISERROR(MATCH(A63,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
       </c>
       <c r="H63" t="b">
-        <f>AND(NOT(G63),F63,IF(D63&lt;&gt;"",VLOOKUP(D63,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>67</v>
       </c>
@@ -2733,22 +2524,22 @@
         <v>69</v>
       </c>
       <c r="E64" t="str">
-        <f>IFERROR(VLOOKUP(C64,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F64" t="b">
-        <f>ISERROR(MATCH(A64,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
       </c>
       <c r="H64" t="e">
-        <f>AND(NOT(G64),F64,IF(D64&lt;&gt;"",VLOOKUP(D64,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>68</v>
       </c>
@@ -2762,22 +2553,22 @@
         <v>67</v>
       </c>
       <c r="E65" t="str">
-        <f>IFERROR(VLOOKUP(C65,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F65" t="b">
-        <f>ISERROR(MATCH(A65,C$2:C$120,0))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
       </c>
       <c r="H65" t="b">
-        <f>AND(NOT(G65),F65,IF(D65&lt;&gt;"",VLOOKUP(D65,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" hidden="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>69</v>
       </c>
@@ -2791,22 +2582,22 @@
         <v>11</v>
       </c>
       <c r="E66" t="str">
-        <f>IFERROR(VLOOKUP(C66,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F66" t="b">
-        <f>ISERROR(MATCH(A66,C$2:C$120,0))</f>
+        <f t="shared" ref="F66:F97" si="7">ISERROR(MATCH(A66,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
       </c>
       <c r="H66" t="b">
-        <f>AND(NOT(G66),F66,IF(D66&lt;&gt;"",VLOOKUP(D66,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" hidden="1">
+        <f t="shared" ref="H66:H97" si="8">AND(NOT(G66),F66,IF(D66&lt;&gt;"",VLOOKUP(D66,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>70</v>
       </c>
@@ -2820,22 +2611,22 @@
         <v>71</v>
       </c>
       <c r="E67" t="str">
-        <f>IFERROR(VLOOKUP(C67,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v>?</v>
       </c>
       <c r="F67" t="b">
-        <f>ISERROR(MATCH(A67,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
       <c r="H67" t="b">
-        <f>AND(NOT(G67),F67,IF(D67&lt;&gt;"",VLOOKUP(D67,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>71</v>
       </c>
@@ -2846,22 +2637,22 @@
         <v>11</v>
       </c>
       <c r="E68" t="str">
-        <f>IFERROR(VLOOKUP(C68,A$2:G$120,5),"")</f>
+        <f t="shared" si="6"/>
         <v>?</v>
       </c>
       <c r="F68" t="b">
-        <f>ISERROR(MATCH(A68,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G68" t="b">
         <v>0</v>
       </c>
       <c r="H68" t="b">
-        <f>AND(NOT(G68),F68,IF(D68&lt;&gt;"",VLOOKUP(D68,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>72</v>
       </c>
@@ -2875,18 +2666,18 @@
         <v>16</v>
       </c>
       <c r="F69" t="b">
-        <f>ISERROR(MATCH(A69,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
       </c>
       <c r="H69" t="b">
-        <f>AND(NOT(G69),F69,IF(D69&lt;&gt;"",VLOOKUP(D69,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>73</v>
       </c>
@@ -2897,22 +2688,22 @@
         <v>72</v>
       </c>
       <c r="E70" t="str">
-        <f>IFERROR(VLOOKUP(C70,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E70:E88" si="9">IFERROR(VLOOKUP(C70,A$2:G$120,5),"")</f>
         <v>?</v>
       </c>
       <c r="F70" t="b">
-        <f>ISERROR(MATCH(A70,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
       </c>
       <c r="H70" t="b">
-        <f>AND(NOT(G70),F70,IF(D70&lt;&gt;"",VLOOKUP(D70,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>74</v>
       </c>
@@ -2923,22 +2714,22 @@
         <v>72</v>
       </c>
       <c r="E71" t="str">
-        <f>IFERROR(VLOOKUP(C71,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v>?</v>
       </c>
       <c r="F71" t="b">
-        <f>ISERROR(MATCH(A71,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G71" t="b">
         <v>0</v>
       </c>
       <c r="H71" t="b">
-        <f>AND(NOT(G71),F71,IF(D71&lt;&gt;"",VLOOKUP(D71,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>75</v>
       </c>
@@ -2952,22 +2743,22 @@
         <v>75</v>
       </c>
       <c r="E72" t="str">
-        <f>IFERROR(VLOOKUP(C72,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v>?</v>
       </c>
       <c r="F72" t="b">
-        <f>ISERROR(MATCH(A72,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
       </c>
       <c r="H72" t="e">
-        <f>AND(NOT(G72),F72,IF(D72&lt;&gt;"",VLOOKUP(D72,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>76</v>
       </c>
@@ -2981,22 +2772,22 @@
         <v>68</v>
       </c>
       <c r="E73" t="str">
-        <f>IFERROR(VLOOKUP(C73,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F73" t="b">
-        <f>ISERROR(MATCH(A73,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G73" t="b">
         <v>0</v>
       </c>
       <c r="H73" t="b">
-        <f>AND(NOT(G73),F73,IF(D73&lt;&gt;"",VLOOKUP(D73,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>77</v>
       </c>
@@ -3010,22 +2801,22 @@
         <v>89</v>
       </c>
       <c r="E74" t="str">
-        <f>IFERROR(VLOOKUP(C74,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F74" t="b">
-        <f>ISERROR(MATCH(A74,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
       </c>
       <c r="H74" t="e">
-        <f>AND(NOT(G74),F74,IF(D74&lt;&gt;"",VLOOKUP(D74,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>78</v>
       </c>
@@ -3039,22 +2830,22 @@
         <v>3</v>
       </c>
       <c r="E75" t="str">
-        <f>IFERROR(VLOOKUP(C75,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F75" t="b">
-        <f>ISERROR(MATCH(A75,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
       </c>
       <c r="H75" t="b">
-        <f>AND(NOT(G75),F75,IF(D75&lt;&gt;"",VLOOKUP(D75,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>79</v>
       </c>
@@ -3065,22 +2856,22 @@
         <v>14</v>
       </c>
       <c r="E76" t="str">
-        <f>IFERROR(VLOOKUP(C76,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F76" t="b">
-        <f>ISERROR(MATCH(A76,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G76" t="b">
         <v>0</v>
       </c>
       <c r="H76" t="b">
-        <f>AND(NOT(G76),F76,IF(D76&lt;&gt;"",VLOOKUP(D76,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>80</v>
       </c>
@@ -3091,22 +2882,22 @@
         <v>2</v>
       </c>
       <c r="E77" t="str">
-        <f>IFERROR(VLOOKUP(C77,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F77" t="b">
-        <f>ISERROR(MATCH(A77,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
       </c>
       <c r="H77" t="b">
-        <f>AND(NOT(G77),F77,IF(D77&lt;&gt;"",VLOOKUP(D77,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>81</v>
       </c>
@@ -3117,22 +2908,22 @@
         <v>102</v>
       </c>
       <c r="E78" t="str">
-        <f>IFERROR(VLOOKUP(C78,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F78" t="b">
-        <f>ISERROR(MATCH(A78,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
       </c>
       <c r="H78" t="b">
-        <f>AND(NOT(G78),F78,IF(D78&lt;&gt;"",VLOOKUP(D78,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>82</v>
       </c>
@@ -3143,22 +2934,22 @@
         <v>81</v>
       </c>
       <c r="E79" t="str">
-        <f>IFERROR(VLOOKUP(C79,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F79" t="b">
-        <f>ISERROR(MATCH(A79,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
       </c>
       <c r="H79" t="b">
-        <f>AND(NOT(G79),F79,IF(D79&lt;&gt;"",VLOOKUP(D79,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>83</v>
       </c>
@@ -3169,22 +2960,22 @@
         <v>81</v>
       </c>
       <c r="E80" t="str">
-        <f>IFERROR(VLOOKUP(C80,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F80" t="b">
-        <f>ISERROR(MATCH(A80,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G80" t="b">
         <v>0</v>
       </c>
       <c r="H80" t="b">
-        <f>AND(NOT(G80),F80,IF(D80&lt;&gt;"",VLOOKUP(D80,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>84</v>
       </c>
@@ -3195,22 +2986,22 @@
         <v>102</v>
       </c>
       <c r="E81" t="str">
-        <f>IFERROR(VLOOKUP(C81,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F81" t="b">
-        <f>ISERROR(MATCH(A81,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G81" t="b">
         <v>0</v>
       </c>
       <c r="H81" t="b">
-        <f>AND(NOT(G81),F81,IF(D81&lt;&gt;"",VLOOKUP(D81,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>86</v>
       </c>
@@ -3221,22 +3012,22 @@
         <v>102</v>
       </c>
       <c r="E82" t="str">
-        <f>IFERROR(VLOOKUP(C82,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F82" t="b">
-        <f>ISERROR(MATCH(A82,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
       </c>
       <c r="H82" t="b">
-        <f>AND(NOT(G82),F82,IF(D82&lt;&gt;"",VLOOKUP(D82,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>87</v>
       </c>
@@ -3250,22 +3041,22 @@
         <v>14</v>
       </c>
       <c r="E83" t="str">
-        <f>IFERROR(VLOOKUP(C83,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F83" t="b">
-        <f>ISERROR(MATCH(A83,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G83" t="b">
         <v>0</v>
       </c>
       <c r="H83" t="b">
-        <f>AND(NOT(G83),F83,IF(D83&lt;&gt;"",VLOOKUP(D83,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>87</v>
       </c>
@@ -3279,22 +3070,22 @@
         <v>22</v>
       </c>
       <c r="E84" t="str">
-        <f>IFERROR(VLOOKUP(C84,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F84" t="b">
-        <f>ISERROR(MATCH(A84,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G84" t="b">
         <v>0</v>
       </c>
       <c r="H84" t="e">
-        <f>AND(NOT(G84),F84,IF(D84&lt;&gt;"",VLOOKUP(D84,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>88</v>
       </c>
@@ -3308,22 +3099,22 @@
         <v>12</v>
       </c>
       <c r="E85" t="str">
-        <f>IFERROR(VLOOKUP(C85,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F85" t="b">
-        <f>ISERROR(MATCH(A85,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
       </c>
       <c r="H85" t="b">
-        <f>AND(NOT(G85),F85,IF(D85&lt;&gt;"",VLOOKUP(D85,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>88</v>
       </c>
@@ -3337,22 +3128,22 @@
         <v>94</v>
       </c>
       <c r="E86" t="str">
-        <f>IFERROR(VLOOKUP(C86,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F86" t="b">
-        <f>ISERROR(MATCH(A86,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G86" t="b">
         <v>0</v>
       </c>
       <c r="H86" t="b">
-        <f>AND(NOT(G86),F86,IF(D86&lt;&gt;"",VLOOKUP(D86,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>89</v>
       </c>
@@ -3366,22 +3157,22 @@
         <v>7</v>
       </c>
       <c r="E87" t="str">
-        <f>IFERROR(VLOOKUP(C87,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F87" t="b">
-        <f>ISERROR(MATCH(A87,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G87" t="b">
         <v>0</v>
       </c>
       <c r="H87" t="b">
-        <f>AND(NOT(G87),F87,IF(D87&lt;&gt;"",VLOOKUP(D87,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>89</v>
       </c>
@@ -3395,22 +3186,22 @@
         <v>12</v>
       </c>
       <c r="E88" t="str">
-        <f>IFERROR(VLOOKUP(C88,A$2:G$120,5),"")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F88" t="b">
-        <f>ISERROR(MATCH(A88,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G88" t="b">
         <v>0</v>
       </c>
       <c r="H88" t="b">
-        <f>AND(NOT(G88),F88,IF(D88&lt;&gt;"",VLOOKUP(D88,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>90</v>
       </c>
@@ -3427,18 +3218,18 @@
         <v>16</v>
       </c>
       <c r="F89" t="b">
-        <f>ISERROR(MATCH(A89,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G89" t="b">
         <v>0</v>
       </c>
       <c r="H89" t="b">
-        <f>AND(NOT(G89),F89,IF(D89&lt;&gt;"",VLOOKUP(D89,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
@@ -3449,22 +3240,22 @@
         <v>89</v>
       </c>
       <c r="E90" t="str">
-        <f>IFERROR(VLOOKUP(C90,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E90:E111" si="10">IFERROR(VLOOKUP(C90,A$2:G$120,5),"")</f>
         <v/>
       </c>
       <c r="F90" t="b">
-        <f>ISERROR(MATCH(A90,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
       </c>
       <c r="H90" t="b">
-        <f>AND(NOT(G90),F90,IF(D90&lt;&gt;"",VLOOKUP(D90,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
@@ -3475,22 +3266,22 @@
         <v>89</v>
       </c>
       <c r="E91" t="str">
-        <f>IFERROR(VLOOKUP(C91,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F91" t="b">
-        <f>ISERROR(MATCH(A91,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" t="b">
-        <f>AND(NOT(G91),F91,IF(D91&lt;&gt;"",VLOOKUP(D91,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3504,22 +3295,22 @@
         <v>14</v>
       </c>
       <c r="E92" t="str">
-        <f>IFERROR(VLOOKUP(C92,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F92" t="b">
-        <f>ISERROR(MATCH(A92,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
       </c>
       <c r="H92" t="b">
-        <f>AND(NOT(G92),F92,IF(D92&lt;&gt;"",VLOOKUP(D92,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3530,22 +3321,22 @@
         <v>121</v>
       </c>
       <c r="E93" t="str">
-        <f>IFERROR(VLOOKUP(C93,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F93" t="b">
-        <f>ISERROR(MATCH(A93,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G93" t="b">
         <v>0</v>
       </c>
       <c r="H93" t="e">
-        <f>AND(NOT(G93),F93,IF(D93&lt;&gt;"",VLOOKUP(D93,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3556,22 +3347,22 @@
         <v>102</v>
       </c>
       <c r="E94" t="str">
-        <f>IFERROR(VLOOKUP(C94,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F94" t="b">
-        <f>ISERROR(MATCH(A94,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G94" t="b">
         <v>0</v>
       </c>
       <c r="H94" t="b">
-        <f>AND(NOT(G94),F94,IF(D94&lt;&gt;"",VLOOKUP(D94,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3582,22 +3373,22 @@
         <v>92</v>
       </c>
       <c r="E95" t="str">
-        <f>IFERROR(VLOOKUP(C95,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F95" t="b">
-        <f>ISERROR(MATCH(A95,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G95" t="b">
         <v>0</v>
       </c>
       <c r="H95" t="b">
-        <f>AND(NOT(G95),F95,IF(D95&lt;&gt;"",VLOOKUP(D95,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3608,22 +3399,22 @@
         <v>92</v>
       </c>
       <c r="E96" t="str">
-        <f>IFERROR(VLOOKUP(C96,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F96" t="b">
-        <f>ISERROR(MATCH(A96,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G96" t="b">
         <v>0</v>
       </c>
       <c r="H96" t="b">
-        <f>AND(NOT(G96),F96,IF(D96&lt;&gt;"",VLOOKUP(D96,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3637,22 +3428,22 @@
         <v>94</v>
       </c>
       <c r="E97" t="str">
-        <f>IFERROR(VLOOKUP(C97,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F97" t="b">
-        <f>ISERROR(MATCH(A97,C$2:C$120,0))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G97" t="b">
         <v>0</v>
       </c>
       <c r="H97" t="b">
-        <f>AND(NOT(G97),F97,IF(D97&lt;&gt;"",VLOOKUP(D97,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" hidden="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3666,22 +3457,22 @@
         <v>95</v>
       </c>
       <c r="E98" t="str">
-        <f>IFERROR(VLOOKUP(C98,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F98" t="b">
-        <f>ISERROR(MATCH(A98,C$2:C$120,0))</f>
+        <f t="shared" ref="F98:F120" si="11">ISERROR(MATCH(A98,C$2:C$120,0))</f>
         <v>1</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
       </c>
       <c r="H98" t="b">
-        <f>AND(NOT(G98),F98,IF(D98&lt;&gt;"",VLOOKUP(D98,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <f t="shared" ref="H98:H129" si="12">AND(NOT(G98),F98,IF(D98&lt;&gt;"",VLOOKUP(D98,A$2:G$120,7),TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3692,22 +3483,22 @@
         <v>37</v>
       </c>
       <c r="E99" t="str">
-        <f>IFERROR(VLOOKUP(C99,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F99" t="b">
-        <f>ISERROR(MATCH(A99,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G99" t="b">
         <v>0</v>
       </c>
       <c r="H99" t="b">
-        <f>AND(NOT(G99),F99,IF(D99&lt;&gt;"",VLOOKUP(D99,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3718,22 +3509,22 @@
         <v>37</v>
       </c>
       <c r="E100" t="str">
-        <f>IFERROR(VLOOKUP(C100,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F100" t="b">
-        <f>ISERROR(MATCH(A100,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G100" t="b">
         <v>0</v>
       </c>
       <c r="H100" t="b">
-        <f>AND(NOT(G100),F100,IF(D100&lt;&gt;"",VLOOKUP(D100,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3744,22 +3535,22 @@
         <v>36</v>
       </c>
       <c r="E101" t="str">
-        <f>IFERROR(VLOOKUP(C101,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F101" t="b">
-        <f>ISERROR(MATCH(A101,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
       </c>
       <c r="H101" t="b">
-        <f>AND(NOT(G101),F101,IF(D101&lt;&gt;"",VLOOKUP(D101,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3770,22 +3561,22 @@
         <v>35</v>
       </c>
       <c r="E102" t="str">
-        <f>IFERROR(VLOOKUP(C102,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F102" t="b">
-        <f>ISERROR(MATCH(A102,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G102" t="b">
         <v>0</v>
       </c>
       <c r="H102" t="b">
-        <f>AND(NOT(G102),F102,IF(D102&lt;&gt;"",VLOOKUP(D102,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -3796,22 +3587,22 @@
         <v>33</v>
       </c>
       <c r="E103" t="str">
-        <f>IFERROR(VLOOKUP(C103,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F103" t="b">
-        <f>ISERROR(MATCH(A103,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G103" t="b">
         <v>0</v>
       </c>
       <c r="H103" t="b">
-        <f>AND(NOT(G103),F103,IF(D103&lt;&gt;"",VLOOKUP(D103,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -3825,22 +3616,22 @@
         <v>100</v>
       </c>
       <c r="E104" t="str">
-        <f>IFERROR(VLOOKUP(C104,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F104" t="b">
-        <f>ISERROR(MATCH(A104,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G104" t="b">
         <v>0</v>
       </c>
       <c r="H104" t="b">
-        <f>AND(NOT(G104),F104,IF(D104&lt;&gt;"",VLOOKUP(D104,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>101</v>
       </c>
@@ -3851,22 +3642,22 @@
         <v>35</v>
       </c>
       <c r="E105" t="str">
-        <f>IFERROR(VLOOKUP(C105,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F105" t="b">
-        <f>ISERROR(MATCH(A105,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G105" t="b">
         <v>0</v>
       </c>
       <c r="H105" t="b">
-        <f>AND(NOT(G105),F105,IF(D105&lt;&gt;"",VLOOKUP(D105,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>102</v>
       </c>
@@ -3874,22 +3665,22 @@
         <v>4</v>
       </c>
       <c r="E106" t="str">
-        <f>IFERROR(VLOOKUP(C106,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F106" t="b">
-        <f>ISERROR(MATCH(A106,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G106" t="b">
         <v>0</v>
       </c>
       <c r="H106" t="b">
-        <f>AND(NOT(G106),F106,IF(D106&lt;&gt;"",VLOOKUP(D106,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>103</v>
       </c>
@@ -3900,22 +3691,22 @@
         <v>102</v>
       </c>
       <c r="E107" t="str">
-        <f>IFERROR(VLOOKUP(C107,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F107" t="b">
-        <f>ISERROR(MATCH(A107,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G107" t="b">
         <v>0</v>
       </c>
       <c r="H107" t="b">
-        <f>AND(NOT(G107),F107,IF(D107&lt;&gt;"",VLOOKUP(D107,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>104</v>
       </c>
@@ -3929,22 +3720,22 @@
         <v>7</v>
       </c>
       <c r="E108" t="str">
-        <f>IFERROR(VLOOKUP(C108,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F108" t="b">
-        <f>ISERROR(MATCH(A108,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G108" t="b">
         <v>0</v>
       </c>
       <c r="H108" t="b">
-        <f>AND(NOT(G108),F108,IF(D108&lt;&gt;"",VLOOKUP(D108,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>105</v>
       </c>
@@ -3952,22 +3743,22 @@
         <v>25</v>
       </c>
       <c r="E109" t="str">
-        <f>IFERROR(VLOOKUP(C109,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F109" t="b">
-        <f>ISERROR(MATCH(A109,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G109" t="b">
         <v>0</v>
       </c>
       <c r="H109" t="b">
-        <f>AND(NOT(G109),F109,IF(D109&lt;&gt;"",VLOOKUP(D109,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>106</v>
       </c>
@@ -3975,22 +3766,22 @@
         <v>65</v>
       </c>
       <c r="E110" t="str">
-        <f>IFERROR(VLOOKUP(C110,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F110" t="b">
-        <f>ISERROR(MATCH(A110,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G110" t="b">
         <v>0</v>
       </c>
       <c r="H110" t="b">
-        <f>AND(NOT(G110),F110,IF(D110&lt;&gt;"",VLOOKUP(D110,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>107</v>
       </c>
@@ -3998,22 +3789,22 @@
         <v>85</v>
       </c>
       <c r="E111" t="str">
-        <f>IFERROR(VLOOKUP(C111,A$2:G$120,5),"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F111" t="b">
-        <f>ISERROR(MATCH(A111,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
       </c>
       <c r="H111" t="b">
-        <f>AND(NOT(G111),F111,IF(D111&lt;&gt;"",VLOOKUP(D111,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>108</v>
       </c>
@@ -4027,18 +3818,18 @@
         <v>16</v>
       </c>
       <c r="F112" t="b">
-        <f>ISERROR(MATCH(A112,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G112" t="b">
         <v>0</v>
       </c>
       <c r="H112" t="b">
-        <f>AND(NOT(G112),F112,IF(D112&lt;&gt;"",VLOOKUP(D112,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>109</v>
       </c>
@@ -4049,22 +3840,22 @@
         <v>102</v>
       </c>
       <c r="E113" t="str">
-        <f>IFERROR(VLOOKUP(C113,A$2:G$120,5),"")</f>
+        <f t="shared" ref="E113:E118" si="13">IFERROR(VLOOKUP(C113,A$2:G$120,5),"")</f>
         <v/>
       </c>
       <c r="F113" t="b">
-        <f>ISERROR(MATCH(A113,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G113" t="b">
         <v>0</v>
       </c>
       <c r="H113" t="b">
-        <f>AND(NOT(G113),F113,IF(D113&lt;&gt;"",VLOOKUP(D113,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>110</v>
       </c>
@@ -4075,22 +3866,22 @@
         <v>109</v>
       </c>
       <c r="E114" t="str">
-        <f>IFERROR(VLOOKUP(C114,A$2:G$120,5),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F114" t="b">
-        <f>ISERROR(MATCH(A114,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G114" t="b">
         <v>0</v>
       </c>
       <c r="H114" t="b">
-        <f>AND(NOT(G114),F114,IF(D114&lt;&gt;"",VLOOKUP(D114,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>111</v>
       </c>
@@ -4101,22 +3892,22 @@
         <v>109</v>
       </c>
       <c r="E115" t="str">
-        <f>IFERROR(VLOOKUP(C115,A$2:G$120,5),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F115" t="b">
-        <f>ISERROR(MATCH(A115,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G115" t="b">
         <v>0</v>
       </c>
       <c r="H115" t="b">
-        <f>AND(NOT(G115),F115,IF(D115&lt;&gt;"",VLOOKUP(D115,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>112</v>
       </c>
@@ -4127,22 +3918,22 @@
         <v>109</v>
       </c>
       <c r="E116" t="str">
-        <f>IFERROR(VLOOKUP(C116,A$2:G$120,5),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F116" t="b">
-        <f>ISERROR(MATCH(A116,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G116" t="b">
         <v>0</v>
       </c>
       <c r="H116" t="b">
-        <f>AND(NOT(G116),F116,IF(D116&lt;&gt;"",VLOOKUP(D116,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>113</v>
       </c>
@@ -4153,22 +3944,22 @@
         <v>109</v>
       </c>
       <c r="E117" t="str">
-        <f>IFERROR(VLOOKUP(C117,A$2:G$120,5),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F117" t="b">
-        <f>ISERROR(MATCH(A117,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G117" t="b">
         <v>0</v>
       </c>
       <c r="H117" t="b">
-        <f>AND(NOT(G117),F117,IF(D117&lt;&gt;"",VLOOKUP(D117,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" hidden="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>114</v>
       </c>
@@ -4182,22 +3973,22 @@
         <v>68</v>
       </c>
       <c r="E118" t="str">
-        <f>IFERROR(VLOOKUP(C118,A$2:G$120,5),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F118" t="b">
-        <f>ISERROR(MATCH(A118,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G118" t="b">
         <v>0</v>
       </c>
       <c r="H118" t="b">
-        <f>AND(NOT(G118),F118,IF(D118&lt;&gt;"",VLOOKUP(D118,A$2:G$120,7),TRUE))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>115</v>
       </c>
@@ -4211,18 +4002,18 @@
         <v>16</v>
       </c>
       <c r="F119" t="b">
-        <f>ISERROR(MATCH(A119,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G119" t="b">
         <v>0</v>
       </c>
       <c r="H119" t="b">
-        <f>AND(NOT(G119),F119,IF(D119&lt;&gt;"",VLOOKUP(D119,A$2:G$120,7),TRUE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>116</v>
       </c>
@@ -4236,25 +4027,19 @@
         <v>16</v>
       </c>
       <c r="F120" t="b">
-        <f>ISERROR(MATCH(A120,C$2:C$120,0))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G120" t="b">
         <v>0</v>
       </c>
       <c r="H120" t="b">
-        <f>AND(NOT(G120),F120,IF(D120&lt;&gt;"",VLOOKUP(D120,A$2:G$120,7),TRUE))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H120">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H120"/>
   <sortState ref="A2:E113">
     <sortCondition ref="A85"/>
   </sortState>
@@ -4275,24 +4060,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>